<commit_message>
updated CI on spreadsheet
</commit_message>
<xml_diff>
--- a/example/KCOR_sample_computation_194x.xlsx
+++ b/example/KCOR_sample_computation_194x.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\KCOR\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF0A6DC-32C4-41D6-B085-641BDA75E70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C519E35D-E3ED-475A-807A-499ED8F39523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_24" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="202">
   <si>
     <t>baseline</t>
   </si>
@@ -660,6 +660,9 @@
   <si>
     <t>this says the same thing:</t>
   </si>
+  <si>
+    <t>for the ASMR computation:</t>
+  </si>
 </sst>
 </file>
 
@@ -9029,7 +9032,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2021_24'!$AL$5</c15:sqref>
@@ -9049,7 +9052,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2021_24'!$AC$6:$AC$168</c15:sqref>
@@ -9552,7 +9555,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2021_24'!$AL$6:$AL$168</c15:sqref>
@@ -10055,7 +10058,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-EDF0-4B42-82AA-3494E71A4B54}"/>
                   </c:ext>
@@ -10421,6 +10424,182 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>199223</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>103842</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEBA6EB7-E735-CAA0-506A-185014F33005}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485775" y="7877175"/>
+          <a:ext cx="6419048" cy="7466667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>18180</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>66384</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7456B336-8A6C-BBC8-8A77-139DA87F3C3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="371475" y="15649575"/>
+          <a:ext cx="6961905" cy="2323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>322949</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>94318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2009A012-D3C7-5FAC-B4A2-098273261CD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7743825" y="66675"/>
+          <a:ext cx="7209524" cy="7457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>37257</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>94405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A0F63C6-AC55-8AC5-0DFB-C81FE35733DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7924800" y="8001000"/>
+          <a:ext cx="6742857" cy="6761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10713,8 +10892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AS32" sqref="AS32"/>
+    <sheetView topLeftCell="U79" workbookViewId="0">
+      <selection activeCell="AE86" sqref="AE86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47619,10 +47798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84728F8-6872-4219-9AA6-EC52FA12A088}">
-  <dimension ref="B16"/>
+  <dimension ref="A16:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47632,6 +47811,11 @@
         <v>200</v>
       </c>
     </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fixed CI bug with ASMR not blanking
</commit_message>
<xml_diff>
--- a/example/KCOR_sample_computation_194x.xlsx
+++ b/example/KCOR_sample_computation_194x.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\KCOR\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C519E35D-E3ED-475A-807A-499ED8F39523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3B5808-52CF-427B-9642-4CC52A9A6DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="2115" windowWidth="22110" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_24" sheetId="1" r:id="rId1"/>
@@ -2871,1034 +2871,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2021_24'!$AF$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>d2/d1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2021_24'!$AC$6:$AC$168</c:f>
-              <c:strCache>
-                <c:ptCount val="163"/>
-                <c:pt idx="0">
-                  <c:v>2021-24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2021-25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2021-26</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2021-27</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2021-28</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2021-29</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2021-30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2021-31</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2021-32</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2021-33</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2021-34</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2021-35</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2021-36</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2021-37</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2021-38</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2021-39</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2021-40</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2021-41</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2021-42</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2021-43</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2021-44</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2021-45</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2021-46</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2021-47</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2021-48</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2021-49</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2021-50</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2021-51</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2021-52</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2022-01</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2022-02</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2022-03</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2022-04</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2022-05</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2022-06</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2022-07</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2022-08</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2022-09</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2022-10</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2022-11</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2022-12</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2022-13</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2022-14</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2022-15</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2022-16</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2022-17</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2022-18</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2022-19</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>2022-20</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2022-21</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2022-22</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2022-23</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2022-24</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2022-25</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2022-26</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2022-27</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>2022-28</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>2022-29</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>2022-30</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>2022-31</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2022-32</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2022-33</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>2022-34</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>2022-35</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>2022-36</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>2022-37</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>2022-38</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>2022-39</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>2022-40</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>2022-41</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>2022-42</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>2022-43</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>2022-44</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>2022-45</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>2022-46</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>2022-47</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>2022-48</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>2022-49</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>2022-50</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>2022-51</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>2022-52</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>2023-01</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>2023-02</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>2023-03</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>2023-04</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>2023-05</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>2023-06</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>2023-07</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>2023-08</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>2023-09</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>2023-10</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>2023-11</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>2023-12</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>2023-13</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>2023-14</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>2023-15</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>2023-16</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>2023-17</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>2023-18</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>2023-19</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>2023-20</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>2023-21</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>2023-22</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>2023-23</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>2023-24</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>2023-25</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>2023-26</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>2023-27</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>2023-28</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>2023-29</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>2023-30</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>2023-31</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>2023-32</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>2023-33</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>2023-34</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>2023-35</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>2023-36</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>2023-37</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>2023-38</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>2023-39</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>2023-40</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>2023-41</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>2023-42</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>2023-43</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>2023-44</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>2023-45</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>2023-46</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>2023-47</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>2023-48</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>2023-49</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>2023-50</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>2023-51</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>2023-52</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>2024-01</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>2024-02</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>2024-03</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>2024-04</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>2024-05</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>2024-06</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>2024-07</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>2024-08</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>2024-09</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>2024-10</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>2024-11</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>2024-12</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>2024-13</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>2024-14</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>2024-15</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>2024-16</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>2024-17</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>2024-18</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>2024-19</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>2024-20</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>2024-21</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>2024-22</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>2024-23</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>2024-24</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>2024-25</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>2024-26</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>2024-27</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>2024-28</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>2024-29</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>2024-30</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2021_24'!$AF$6:$AF$168</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="163"/>
-                <c:pt idx="0">
-                  <c:v>0.91179765951377534</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.98453628099064605</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94683392711182923</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.95960611794087858</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.9975139755677469</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0217304790872073</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0194055859460918</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0248965093000768</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0327584160111143</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.034223471733501</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.0431081674181226</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.0460065368100044</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.0387667204580948</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.0493330430285612</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.0459176219915596</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.0398566821951967</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.0515859109379269</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.0634782301901529</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.0753132615844168</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.087213457703464</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.0853319943255351</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.0898931151297961</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.0927599134120618</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.0946774000863941</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.0974536719577346</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.0994853759377166</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.1019649385152321</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.1008831678687554</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.1050776635838038</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.1065710193265788</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.105981038111002</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1.1054073855014723</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.1097610020710722</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.1097366047302566</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.1086463352859381</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.1103365905283982</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.1162499311639775</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.1194648541604502</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.1277368058797437</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.1221620988557481</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.1243776232676335</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.1240908444146902</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.1219688733172539</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.1237073512236269</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1.1270785242758496</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.1274360658020859</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1.1355816289088059</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.131526979130304</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1.1294829468155607</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1.1296900827704353</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1.1308585216852811</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1.1324709870785026</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1.1347781102898047</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1.1371346970731817</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1.1362425805116494</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>1.1361156258364009</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>1.1385530737290694</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1.138323140382564</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1.1419583253007544</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1.1405227189127307</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>1.1394036600432775</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1.1405046653433994</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>1.1411007718244885</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1.1424478290380289</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1.1459638844525186</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1.1442343786882878</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>1.143515388199738</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1.1423931151880216</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1.144485427257663</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1.1448459856927655</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1.147225531535492</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1.1475238053733428</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1.147895247016153</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1.1463765390091665</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1.1479971618018892</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>1.1489114789872799</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1.1460415220791886</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1.1446624699403303</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1.14545041062705</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1.145450651179871</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1.1463729800876461</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1.1445424690039572</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>1.1428951165050396</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1.1408243085247867</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1.143790759031925</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>1.1432408676998522</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>1.1415213719847193</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>1.1419140475969762</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>1.1430146095805649</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>1.1413709511023122</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>1.1417012592457578</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>1.142498178259665</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1.1436519864756756</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>1.1431968953874083</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1.1418983793342423</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>1.1408624264393235</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>1.14033416495481</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>1.1402038135535093</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>1.1403342075808383</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>1.1394071708380735</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>1.1396334367591354</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>1.1388419890573616</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>1.1390179461872942</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>1.1397386781844285</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>1.1403814818926108</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>1.1408428974643439</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>1.1414626954882074</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>1.1422624099119958</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>1.1432938742695209</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>1.1427473938984707</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>1.1433950922273459</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>1.1427921513278683</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>1.1435119950339347</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>1.1430783865771004</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>1.143679186472391</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>1.1438452778230215</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>1.1456213519917273</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>1.1449659395163336</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>1.146571034686916</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>1.1472165050716825</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>1.1464889259406992</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>1.1457838180284245</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>1.1460507290932438</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>1.1449412536797765</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>1.1445140493475505</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>1.1437052936655361</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>1.142817630991102</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>1.1423324074863479</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>1.1409385141605286</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>1.1417847975691047</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>1.1408528319214954</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>1.1410997498802851</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>1.1403819427331316</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>1.1415494671881976</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>1.1416950151251883</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>1.1410410378894251</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>1.1414741704680984</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>1.1409857900474374</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>1.141135456966575</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>1.1385326776704212</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>1.1368937253569276</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>1.1379392394504231</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>1.1390275742553428</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>1.1387785434802824</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>1.1377466340225832</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>1.1369488828194128</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>1.1352606318368119</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>1.1355595540886609</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>1.1363613762897387</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>1.1360395571496729</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>1.1365220125163247</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>1.1367798619221281</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>1.1361405381510878</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>1.1369790660323631</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>1.1366241647592883</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>1.1361684150266655</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>1.1363254150312727</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>1.1368175328230639</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>1.1378749386532652</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>1.1375530781272418</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>1.136895059776226</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>1.1362367213210418</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-EDF0-4B42-82AA-3494E71A4B54}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
@@ -4419,19 +3391,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="163"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.82249265850892694</c:v>
@@ -5438,19 +4410,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="163"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.2979736142846487</c:v>
@@ -6457,19 +5429,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="163"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.85861392228206745</c:v>
@@ -7476,19 +6448,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="163"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.2371944014889749</c:v>
@@ -7989,25 +6961,34 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="7"/>
-                <c:order val="7"/>
+                <c:idx val="2"/>
+                <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'2021_24'!$AK$5</c15:sqref>
+                          <c15:sqref>'2021_24'!$AF$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>CI low d2/d1</c:v>
+                        <c:v>d2/d1</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:prstDash val="solid"/>
+                    <a:round/>
+                  </a:ln>
+                </c:spPr>
                 <c:marker>
                   <c:symbol val="none"/>
                 </c:marker>
@@ -8519,6 +7500,1045 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
+                          <c15:sqref>'2021_24'!$AF$6:$AF$168</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="163"/>
+                      <c:pt idx="0">
+                        <c:v>0.91179765951377534</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.98453628099064605</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.94683392711182923</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.95960611794087858</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.9975139755677469</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.0217304790872073</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.0194055859460918</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1.0248965093000768</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1.0327584160111143</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.034223471733501</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1.0431081674181226</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1.0460065368100044</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>1.0387667204580948</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>1.0493330430285612</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>1.0459176219915596</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1.0398566821951967</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>1.0515859109379269</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>1.0634782301901529</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>1.0753132615844168</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>1.087213457703464</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>1.0853319943255351</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>1.0898931151297961</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>1.0927599134120618</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>1.0946774000863941</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>1.0974536719577346</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>1.0994853759377166</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>1.1019649385152321</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>1.1008831678687554</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>1.1050776635838038</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>1.1065710193265788</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>1.105981038111002</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>1.1054073855014723</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>1.1097610020710722</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>1.1097366047302566</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>1.1086463352859381</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>1.1103365905283982</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>1.1162499311639775</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>1.1194648541604502</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>1.1277368058797437</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>1.1221620988557481</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>1.1243776232676335</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>1.1240908444146902</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>1.1219688733172539</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>1.1237073512236269</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>1.1270785242758496</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>1.1274360658020859</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>1.1355816289088059</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>1.131526979130304</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>1.1294829468155607</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>1.1296900827704353</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>1.1308585216852811</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>1.1324709870785026</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>1.1347781102898047</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>1.1371346970731817</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>1.1362425805116494</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>1.1361156258364009</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>1.1385530737290694</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>1.138323140382564</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>1.1419583253007544</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>1.1405227189127307</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>1.1394036600432775</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>1.1405046653433994</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>1.1411007718244885</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>1.1424478290380289</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>1.1459638844525186</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>1.1442343786882878</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>1.143515388199738</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>1.1423931151880216</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>1.144485427257663</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>1.1448459856927655</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>1.147225531535492</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>1.1475238053733428</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>1.147895247016153</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>1.1463765390091665</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>1.1479971618018892</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>1.1489114789872799</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>1.1460415220791886</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>1.1446624699403303</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>1.14545041062705</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>1.145450651179871</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>1.1463729800876461</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>1.1445424690039572</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>1.1428951165050396</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>1.1408243085247867</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>1.143790759031925</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>1.1432408676998522</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>1.1415213719847193</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>1.1419140475969762</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>1.1430146095805649</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>1.1413709511023122</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>1.1417012592457578</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>1.142498178259665</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>1.1436519864756756</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>1.1431968953874083</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>1.1418983793342423</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>1.1408624264393235</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>1.14033416495481</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>1.1402038135535093</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>1.1403342075808383</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>1.1394071708380735</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>1.1396334367591354</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>1.1388419890573616</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>1.1390179461872942</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>1.1397386781844285</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>1.1403814818926108</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>1.1408428974643439</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>1.1414626954882074</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>1.1422624099119958</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>1.1432938742695209</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>1.1427473938984707</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>1.1433950922273459</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>1.1427921513278683</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>1.1435119950339347</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>1.1430783865771004</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>1.143679186472391</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>1.1438452778230215</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>1.1456213519917273</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>1.1449659395163336</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>1.146571034686916</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>1.1472165050716825</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>1.1464889259406992</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>1.1457838180284245</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>1.1460507290932438</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>1.1449412536797765</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>1.1445140493475505</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>1.1437052936655361</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>1.142817630991102</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>1.1423324074863479</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>1.1409385141605286</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>1.1417847975691047</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>1.1408528319214954</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>1.1410997498802851</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>1.1403819427331316</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>1.1415494671881976</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>1.1416950151251883</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>1.1410410378894251</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>1.1414741704680984</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>1.1409857900474374</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>1.141135456966575</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>1.1385326776704212</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>1.1368937253569276</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>1.1379392394504231</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>1.1390275742553428</c:v>
+                      </c:pt>
+                      <c:pt idx="144">
+                        <c:v>1.1387785434802824</c:v>
+                      </c:pt>
+                      <c:pt idx="145">
+                        <c:v>1.1377466340225832</c:v>
+                      </c:pt>
+                      <c:pt idx="146">
+                        <c:v>1.1369488828194128</c:v>
+                      </c:pt>
+                      <c:pt idx="147">
+                        <c:v>1.1352606318368119</c:v>
+                      </c:pt>
+                      <c:pt idx="148">
+                        <c:v>1.1355595540886609</c:v>
+                      </c:pt>
+                      <c:pt idx="149">
+                        <c:v>1.1363613762897387</c:v>
+                      </c:pt>
+                      <c:pt idx="150">
+                        <c:v>1.1360395571496729</c:v>
+                      </c:pt>
+                      <c:pt idx="151">
+                        <c:v>1.1365220125163247</c:v>
+                      </c:pt>
+                      <c:pt idx="152">
+                        <c:v>1.1367798619221281</c:v>
+                      </c:pt>
+                      <c:pt idx="153">
+                        <c:v>1.1361405381510878</c:v>
+                      </c:pt>
+                      <c:pt idx="154">
+                        <c:v>1.1369790660323631</c:v>
+                      </c:pt>
+                      <c:pt idx="155">
+                        <c:v>1.1366241647592883</c:v>
+                      </c:pt>
+                      <c:pt idx="156">
+                        <c:v>1.1361684150266655</c:v>
+                      </c:pt>
+                      <c:pt idx="157">
+                        <c:v>1.1363254150312727</c:v>
+                      </c:pt>
+                      <c:pt idx="158">
+                        <c:v>1.1368175328230639</c:v>
+                      </c:pt>
+                      <c:pt idx="159">
+                        <c:v>1.1378749386532652</c:v>
+                      </c:pt>
+                      <c:pt idx="160">
+                        <c:v>1.1375530781272418</c:v>
+                      </c:pt>
+                      <c:pt idx="161">
+                        <c:v>1.136895059776226</c:v>
+                      </c:pt>
+                      <c:pt idx="162">
+                        <c:v>1.1362367213210418</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-EDF0-4B42-82AA-3494E71A4B54}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="7"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'2021_24'!$AK$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>CI low d2/d1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'2021_24'!$AC$6:$AC$168</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="163"/>
+                      <c:pt idx="0">
+                        <c:v>2021-24</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2021-25</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2021-26</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2021-27</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2021-28</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2021-29</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2021-30</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2021-31</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2021-32</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2021-33</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>2021-34</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2021-35</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2021-36</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>2021-37</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>2021-38</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2021-39</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>2021-40</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>2021-41</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>2021-42</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>2021-43</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2021-44</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>2021-45</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2021-46</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>2021-47</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>2021-48</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>2021-49</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>2021-50</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>2021-51</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>2021-52</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>2022-01</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>2022-02</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>2022-03</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>2022-04</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>2022-05</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>2022-06</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>2022-07</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>2022-08</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>2022-09</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>2022-10</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>2022-11</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>2022-12</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>2022-13</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>2022-14</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>2022-15</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>2022-16</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>2022-17</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>2022-18</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>2022-19</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>2022-20</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>2022-21</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>2022-22</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>2022-23</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>2022-24</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>2022-25</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>2022-26</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>2022-27</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>2022-28</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>2022-29</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>2022-30</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>2022-31</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>2022-32</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>2022-33</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>2022-34</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>2022-35</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>2022-36</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>2022-37</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>2022-38</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>2022-39</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>2022-40</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>2022-41</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>2022-42</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>2022-43</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>2022-44</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>2022-45</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>2022-46</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>2022-47</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>2022-48</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>2022-49</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>2022-50</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>2022-51</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>2022-52</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>2023-01</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>2023-02</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>2023-03</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>2023-04</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>2023-05</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>2023-06</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>2023-07</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>2023-08</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>2023-09</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>2023-10</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>2023-11</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>2023-12</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>2023-13</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>2023-14</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>2023-15</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>2023-16</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>2023-17</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>2023-18</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>2023-19</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>2023-20</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>2023-21</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>2023-22</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>2023-23</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>2023-24</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>2023-25</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>2023-26</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>2023-27</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>2023-28</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>2023-29</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>2023-30</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>2023-31</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>2023-32</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>2023-33</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>2023-34</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>2023-35</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>2023-36</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>2023-37</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>2023-38</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>2023-39</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>2023-40</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>2023-41</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>2023-42</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>2023-43</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>2023-44</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>2023-45</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>2023-46</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>2023-47</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>2023-48</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>2023-49</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>2023-50</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>2023-51</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>2023-52</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>2024-01</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>2024-02</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>2024-03</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>2024-04</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>2024-05</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>2024-06</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>2024-07</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>2024-08</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>2024-09</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>2024-10</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>2024-11</c:v>
+                      </c:pt>
+                      <c:pt idx="144">
+                        <c:v>2024-12</c:v>
+                      </c:pt>
+                      <c:pt idx="145">
+                        <c:v>2024-13</c:v>
+                      </c:pt>
+                      <c:pt idx="146">
+                        <c:v>2024-14</c:v>
+                      </c:pt>
+                      <c:pt idx="147">
+                        <c:v>2024-15</c:v>
+                      </c:pt>
+                      <c:pt idx="148">
+                        <c:v>2024-16</c:v>
+                      </c:pt>
+                      <c:pt idx="149">
+                        <c:v>2024-17</c:v>
+                      </c:pt>
+                      <c:pt idx="150">
+                        <c:v>2024-18</c:v>
+                      </c:pt>
+                      <c:pt idx="151">
+                        <c:v>2024-19</c:v>
+                      </c:pt>
+                      <c:pt idx="152">
+                        <c:v>2024-20</c:v>
+                      </c:pt>
+                      <c:pt idx="153">
+                        <c:v>2024-21</c:v>
+                      </c:pt>
+                      <c:pt idx="154">
+                        <c:v>2024-22</c:v>
+                      </c:pt>
+                      <c:pt idx="155">
+                        <c:v>2024-23</c:v>
+                      </c:pt>
+                      <c:pt idx="156">
+                        <c:v>2024-24</c:v>
+                      </c:pt>
+                      <c:pt idx="157">
+                        <c:v>2024-25</c:v>
+                      </c:pt>
+                      <c:pt idx="158">
+                        <c:v>2024-26</c:v>
+                      </c:pt>
+                      <c:pt idx="159">
+                        <c:v>2024-27</c:v>
+                      </c:pt>
+                      <c:pt idx="160">
+                        <c:v>2024-28</c:v>
+                      </c:pt>
+                      <c:pt idx="161">
+                        <c:v>2024-29</c:v>
+                      </c:pt>
+                      <c:pt idx="162">
+                        <c:v>2024-30</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
                           <c15:sqref>'2021_24'!$AK$6:$AK$168</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
@@ -8527,19 +8547,19 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="163"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>0.8000226093877969</c:v>
@@ -9019,7 +9039,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-EDF0-4B42-82AA-3494E71A4B54}"/>
                   </c:ext>
@@ -9032,7 +9052,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2021_24'!$AL$5</c15:sqref>
@@ -9052,7 +9072,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2021_24'!$AC$6:$AC$168</c15:sqref>
@@ -9555,7 +9575,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'2021_24'!$AL$6:$AL$168</c15:sqref>
@@ -9566,19 +9586,19 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="163"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>#N/A</c:v>
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>1.2437575135712775</c:v>
@@ -10298,7 +10318,15 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" kern="1200"/>
-            <a:t>The net harm is statisitically</a:t>
+            <a:t>The net harm by end of 2022</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" kern="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" kern="1200"/>
+            <a:t>is statisitically</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" kern="1200" baseline="0"/>
@@ -10324,7 +10352,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" kern="1200" baseline="0"/>
-            <a:t> age, they have higher mortality and frailty--&gt; greater impact of COVID.</a:t>
+            <a:t> age, they have higher mortality and frailty--&gt; greater impact of COVID. The COVID vaccine had little to no impact. It was primarily selection bias.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200" b="0" kern="1200"/>
         </a:p>
@@ -10892,8 +10920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL168"/>
   <sheetViews>
-    <sheetView topLeftCell="U79" workbookViewId="0">
-      <selection activeCell="AE86" sqref="AE86"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="BF9" sqref="BF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11213,131 +11241,29 @@
         <f t="shared" ref="AF6:AF37" ca="1" si="15">AA6/OFFSET(AA$6,$B$1,0)</f>
         <v>0.91179765951377534</v>
       </c>
-      <c r="AG6" t="str" cm="1">
-        <f t="array" ref="AG6">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AH6" t="str" cm="1">
-        <f t="array" ref="AH6">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AI6" t="str" cm="1">
-        <f t="array" ref="AI6">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AJ6" t="str" cm="1">
-        <f t="array" ref="AJ6">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AK6" t="str" cm="1">
-        <f t="array" ref="AK6">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AL6" t="str" cm="1">
-        <f t="array" ref="AL6">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
+      <c r="AG6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AI6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AK6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AL6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
@@ -11438,131 +11364,29 @@
         <f t="shared" ca="1" si="15"/>
         <v>0.98453628099064605</v>
       </c>
-      <c r="AG7" t="str" cm="1">
-        <f t="array" ref="AG7">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AH7" t="str" cm="1">
-        <f t="array" ref="AH7">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AI7" t="str" cm="1">
-        <f t="array" ref="AI7">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AJ7" t="str" cm="1">
-        <f t="array" ref="AJ7">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AK7" t="str" cm="1">
-        <f t="array" ref="AK7">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AL7" t="str" cm="1">
-        <f t="array" ref="AL7">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
+      <c r="AG7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AI7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AK7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AL7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
@@ -11663,131 +11487,29 @@
         <f t="shared" ca="1" si="15"/>
         <v>0.94683392711182923</v>
       </c>
-      <c r="AG8" t="str" cm="1">
-        <f t="array" ref="AG8">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AH8" t="str" cm="1">
-        <f t="array" ref="AH8">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AI8" t="str" cm="1">
-        <f t="array" ref="AI8">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AJ8" t="str" cm="1">
-        <f t="array" ref="AJ8">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AK8" t="str" cm="1">
-        <f t="array" ref="AK8">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AL8" t="str" cm="1">
-        <f t="array" ref="AL8">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
+      <c r="AG8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AI8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AK8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AL8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -11888,131 +11610,29 @@
         <f t="shared" ca="1" si="15"/>
         <v>0.95960611794087858</v>
       </c>
-      <c r="AG9" t="str" cm="1">
-        <f t="array" ref="AG9">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AH9" t="str" cm="1">
-        <f t="array" ref="AH9">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AI9" t="str" cm="1">
-        <f t="array" ref="AI9">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AJ9" t="str" cm="1">
-        <f t="array" ref="AJ9">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AK9" t="str" cm="1">
-        <f t="array" ref="AK9">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AL9" t="str" cm="1">
-        <f t="array" ref="AL9">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
+      <c r="AG9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AI9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AK9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AL9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -12113,131 +11733,29 @@
         <f t="shared" ca="1" si="15"/>
         <v>1</v>
       </c>
-      <c r="AG10" t="str" cm="1">
-        <f t="array" ref="AG10">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AH10" t="str" cm="1">
-        <f t="array" ref="AH10">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dV^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AD:AD,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AI10" t="str" cm="1">
-        <f t="array" ref="AI10">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AJ10" t="str" cm="1">
-        <f t="array" ref="AJ10">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dU, INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incU, INDEX(U:U,_xlpm.s):INDEX(U:U,_xlpm.r)-INDEX(U:U,_xlpm.t0):INDEX(U:U,_xlpm.r-1),
-    _xlpm.rawU, -LN(1 - INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(E:E,_xlpm.s):INDEX(E:E,_xlpm.r)/(INDEX(B:B,_xlpm.s):INDEX(B:B,_xlpm.r))^2 * (_xlpm.incU/_xlpm.rawU)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dU^2) ),
-    _xlpm.K, INDEX(AE:AE,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AK10" t="str" cm="1">
-        <f t="array" ref="AK10">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K/_xlpm.F
-  )
-)</f>
-        <v/>
-      </c>
-      <c r="AL10" t="str" cm="1">
-        <f t="array" ref="AL10">IF(ROW()&lt;=$B$1+6,"",
-  _xlfn.LET(
-    _xlpm.r,ROW(),
-    _xlpm.t0,$B$1+6, _xlpm.s,$B$1+7,
-    _xlpm.dW, INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0),
-    _xlpm.dV, INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0),
-    _xlpm.incW, INDEX(W:W,_xlpm.s):INDEX(W:W,_xlpm.r)-INDEX(W:W,_xlpm.t0):INDEX(W:W,_xlpm.r-1),
-    _xlpm.rawW, -LN(1 - INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r)),
-    _xlpm.incV, INDEX(V:V,_xlpm.s):INDEX(V:V,_xlpm.r)-INDEX(V:V,_xlpm.t0):INDEX(V:V,_xlpm.r-1),
-    _xlpm.rawV, -LN(1 - INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r)),
-    _xlpm.VarT, SUMPRODUCT( INDEX(G:G,_xlpm.s):INDEX(G:G,_xlpm.r)/(INDEX(D:D,_xlpm.s):INDEX(D:D,_xlpm.r))^2 * (_xlpm.incW/_xlpm.rawW)^2 ),
-    _xlpm.VarU, SUMPRODUCT( INDEX(F:F,_xlpm.s):INDEX(F:F,_xlpm.r)/(INDEX(C:C,_xlpm.s):INDEX(C:C,_xlpm.r))^2 * (_xlpm.incV/_xlpm.rawV)^2 ),
-    _xlpm.SE, SQRT( _xlpm.VarT/(_xlpm.dW^2) + _xlpm.VarU/(_xlpm.dV^2) ),
-    _xlpm.K, INDEX(AF:AF,_xlpm.r),
-    _xlpm.F, EXP(1.96*_xlpm.SE),
-    _xlpm.K*_xlpm.F
-  )
-)</f>
-        <v/>
+      <c r="AG10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AI10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AK10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AL10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -47800,7 +47318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84728F8-6872-4219-9AA6-EC52FA12A088}">
   <dimension ref="A16:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updaed to look at mfg for dose 2 3 and 4
</commit_message>
<xml_diff>
--- a/example/KCOR_sample_computation_194x.xlsx
+++ b/example/KCOR_sample_computation_194x.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\KCOR\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE304B8E-03D5-44AB-91F7-718C1DC83779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5CBB2D-479D-4DAB-B931-9F944C0D3BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="205">
   <si>
     <t>baseline</t>
   </si>
@@ -655,9 +655,6 @@
     <t>Grok validation of the CI formula below</t>
   </si>
   <si>
-    <t>MR computation</t>
-  </si>
-  <si>
     <t>MR=mortality risk (aka interval prob of risk)</t>
   </si>
   <si>
@@ -668,6 +665,12 @@
   </si>
   <si>
     <t>Net impact 1 vs 2 shots</t>
+  </si>
+  <si>
+    <t>h(t) = "instantaneous death rate" aka</t>
+  </si>
+  <si>
+    <t>MR=deaths/(alive at start of interval)</t>
   </si>
 </sst>
 </file>
@@ -11071,7 +11074,7 @@
   <dimension ref="A1:AL168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11103,7 +11106,7 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J1" s="7">
         <f ca="1">AD86</f>
@@ -11157,7 +11160,10 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>200</v>
+        <v>199</v>
+      </c>
+      <c r="M3" t="s">
+        <v>203</v>
       </c>
       <c r="AD3" t="s">
         <v>7</v>
@@ -11168,13 +11174,13 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="I4" s="3" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -11186,7 +11192,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>

</xml_diff>